<commit_message>
Atualização da ATA do dia 23
</commit_message>
<xml_diff>
--- a/Documentação/Gestão/Ata - Sprint 3 - Strawtech.xlsx
+++ b/Documentação/Gestão/Ata - Sprint 3 - Strawtech.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1700239791" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1700239791" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1700239791" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1700239791"/>
+      <pm:revision xmlns:pm="smNativeData" day="1700834835" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1700834835" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1700834835" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1700834835"/>
     </ext>
   </extLst>
 </workbook>
@@ -40,12 +40,18 @@
     <comment ref="F11" authorId="0">
       <text/>
     </comment>
+    <comment ref="F13" authorId="0">
+      <text/>
+    </comment>
+    <comment ref="F15" authorId="0">
+      <text/>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>ATA - PROJETO STRAWTECH</t>
   </si>
@@ -68,6 +74,9 @@
     <t>Assuntos discutidos e principais decisões :</t>
   </si>
   <si>
+    <t>06/11</t>
+  </si>
+  <si>
     <t>Gustavo Bueno
 Gustavo Fernandes
 Pablo Vinícius
@@ -85,6 +94,9 @@
 </t>
   </si>
   <si>
+    <t>07/11</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gustavo Bueno
 Gustavo Fernandes
 Pablo Vinícius
@@ -99,19 +111,31 @@
 •  Foi definidio que o Gustavo F. Será o scrum master dessa semana</t>
   </si>
   <si>
+    <t>08/11</t>
+  </si>
+  <si>
     <t>•  Foi definido que o José irá ajustar o trello e a modelagem do banco de dados.
 •  Foi atualizado o Plano de ação.
 • Foi definido que o Gustavo Fernandes ficará responsável pela integração da ferramneta help Desk e a criação de um novo repositório para a Sprint 3</t>
+  </si>
+  <si>
+    <t>09/11</t>
   </si>
   <si>
     <t xml:space="preserve">•  Foi debatido a prioziação dos intregaveis. 
   </t>
   </si>
   <si>
+    <t>10/11</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 • Foi definido que o Pablo ficara reponsavel pela implementação da web-data-viz.
 • Foi definido que o José ira atualizar o banco 
 </t>
+  </si>
+  <si>
+    <t>13/11</t>
   </si>
   <si>
     <t xml:space="preserve">Gustavo Bueno
@@ -129,8 +153,14 @@
 </t>
   </si>
   <si>
+    <t>14/11</t>
+  </si>
+  <si>
     <t>• Foi defimido que o grupo não ira utilizar a API de criptografia.
 •  Foi atualizado o trello em grupo</t>
+  </si>
+  <si>
+    <t>16/11</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -138,12 +168,29 @@
 • Foi aprensentada a feerramneta Help Desk
 •  Gustavo Fernandes ficou responsável pelo Analytics</t>
   </si>
+  <si>
+    <t>• Foi definido que o Gutavo F. será o Product Owner desta semana.
+• Foi definido que o José  será o Scrum Master desta semana.
+• Foi realizada uma análise com os membros do grupo sobre todo  o desempenho do projeto até o presente momento e foi alinhado tudo o que será necessário ser feito para a entrega do projeto.</t>
+  </si>
+  <si>
+    <t>21/11</t>
+  </si>
+  <si>
+    <t>• Foi alinhado com o grupo o desempenho de cada um dos membros ao longo da semana.</t>
+  </si>
+  <si>
+    <t>22/11</t>
+  </si>
+  <si>
+    <t>23/11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
+  <numFmts count="15">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;R$&quot;;\-#,##0\ &quot;R$&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;R$&quot;;[Red]\-#,##0\ &quot;R$&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;R$&quot;;\-#,##0.00\ &quot;R$&quot;"/>
@@ -158,6 +205,7 @@
     <numFmt numFmtId="49" formatCode="@"/>
     <numFmt numFmtId="164" formatCode="DD/ MMM "/>
     <numFmt numFmtId="165" formatCode="DD/MM"/>
+    <numFmt numFmtId="4" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -167,7 +215,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -182,7 +230,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Verdana" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -196,7 +244,7 @@
       <sz val="49"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Merriweather" sz="980" lang="default"/>
             <pm:cs face="Times New Roman" sz="980" lang="default"/>
             <pm:ea face="SimSun" sz="980" lang="default"/>
@@ -210,7 +258,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Merriweather" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -224,7 +272,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Merriweather" sz="180" lang="default"/>
             <pm:cs face="Times New Roman" sz="180" lang="default"/>
             <pm:ea face="SimSun" sz="180" lang="default"/>
@@ -238,7 +286,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Merriweather" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -253,7 +301,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Verdana" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -268,7 +316,7 @@
       <sz val="9"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1700239791" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1700834835" ulstyle="none" kern="1">
             <pm:latin face="Verdana" sz="180" lang="default"/>
             <pm:cs face="Times New Roman" sz="180" lang="default"/>
             <pm:ea face="SimSun" sz="180" lang="default"/>
@@ -308,7 +356,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FF6D01" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FF6D01" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -319,7 +367,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFE6DD" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFE6DD" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -330,7 +378,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -341,7 +389,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -352,7 +400,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -363,7 +411,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -374,7 +422,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -385,7 +433,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00F46524" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00F46524" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -396,7 +444,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00F46524" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00F46524" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -407,7 +455,18 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE6DD"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFE6DD" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -418,18 +477,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE6DD"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1700239791" type="1" fgLvl="100" fgClr="00FFE6DD" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1700834835" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -451,7 +499,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791"/>
+          <pm:border xmlns:pm="smNativeData" id="1700834835"/>
         </ext>
       </extLst>
     </border>
@@ -470,7 +518,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
@@ -494,7 +542,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
@@ -517,7 +565,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
@@ -540,7 +588,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
@@ -563,7 +611,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -586,7 +634,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
           </pm:border>
@@ -608,7 +656,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -630,7 +678,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -652,7 +700,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -674,7 +722,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -696,7 +744,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -719,7 +767,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
           </pm:border>
@@ -741,7 +789,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="FFFFFF"/>
@@ -764,7 +812,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -785,7 +833,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791">
+          <pm:border xmlns:pm="smNativeData" id="1700834835">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -807,7 +855,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791"/>
+          <pm:border xmlns:pm="smNativeData" id="1700834835"/>
         </ext>
       </extLst>
     </border>
@@ -826,7 +874,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791"/>
+          <pm:border xmlns:pm="smNativeData" id="1700834835"/>
         </ext>
       </extLst>
     </border>
@@ -845,7 +893,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1700239791"/>
+          <pm:border xmlns:pm="smNativeData" id="1700834835"/>
         </ext>
       </extLst>
     </border>
@@ -853,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -882,9 +930,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -892,9 +937,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="3" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -906,25 +948,13 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="6" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -980,16 +1010,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -999,10 +1038,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1700239791" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1700834835" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1700239791" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1700834835" count="3">
         <pm:color name="Cor 24" rgb="FF6D01"/>
         <pm:color name="Cor 25" rgb="F46524"/>
         <pm:color name="Cor 26" rgb="FFE6DD"/>
@@ -1273,13 +1312,13 @@
   </sheetPr>
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A10" zoomScale="71" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A13" zoomScale="71" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="11" defaultColWidth="12.567568" defaultRowHeight="13.45"/>
   <cols>
-    <col min="2" max="2" width="14.423423" customWidth="1"/>
+    <col min="2" max="2" width="18.630631" customWidth="1"/>
     <col min="3" max="3" width="20.711712" customWidth="1"/>
     <col min="4" max="4" width="15.423423" customWidth="1"/>
     <col min="5" max="5" width="26.855856" customWidth="1"/>
@@ -1316,14 +1355,14 @@
     </row>
     <row r="2" spans="1:25" ht="66.75" customHeight="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -1384,23 +1423,23 @@
     </row>
     <row r="4" spans="1:25" ht="111.75" customHeight="1">
       <c r="A4" s="7"/>
-      <c r="B4" s="10" t="n">
-        <v>45236</v>
+      <c r="B4" s="40" t="s">
+        <v>7</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="10" t="n">
         <v>0.416666666666666607</v>
       </c>
-      <c r="D4" s="11" t="n">
-        <v>0.429166666666666696</v>
+      <c r="D4" s="10" t="n">
+        <v>0.429166666666666607</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>9</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -1423,23 +1462,23 @@
     </row>
     <row r="5" spans="1:25" ht="75" customHeight="1">
       <c r="A5" s="7"/>
-      <c r="B5" s="14" t="n">
-        <v>45237</v>
+      <c r="B5" s="41" t="s">
+        <v>11</v>
       </c>
-      <c r="C5" s="15" t="n">
+      <c r="C5" s="13" t="n">
         <v>0.416666666666666607</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="13" t="n">
         <v>0.42638888888888884</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>10</v>
+      <c r="E5" s="14" t="s">
+        <v>12</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>8</v>
+      <c r="F5" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="G5" s="17" t="s">
-        <v>11</v>
+      <c r="G5" s="15" t="s">
+        <v>13</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -1462,23 +1501,23 @@
     </row>
     <row r="6" spans="1:25" ht="135.75" customHeight="1">
       <c r="A6" s="7"/>
-      <c r="B6" s="10" t="n">
-        <v>45238</v>
+      <c r="B6" s="40" t="s">
+        <v>14</v>
       </c>
-      <c r="C6" s="11" t="n">
+      <c r="C6" s="10" t="n">
         <v>0.409722222222222321</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="10" t="n">
         <v>0.425</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>12</v>
+      <c r="F6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -1501,23 +1540,23 @@
     </row>
     <row r="7" spans="1:25" ht="132" customHeight="1">
       <c r="A7" s="7"/>
-      <c r="B7" s="14" t="n">
-        <v>45239</v>
+      <c r="B7" s="41" t="s">
+        <v>16</v>
       </c>
-      <c r="C7" s="15" t="n">
-        <v>0.791666666666666607</v>
+      <c r="C7" s="13" t="n">
+        <v>0.791666666666666519</v>
       </c>
-      <c r="D7" s="15" t="n">
-        <v>0.800694444444444464</v>
+      <c r="D7" s="13" t="n">
+        <v>0.800694444444444287</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>10</v>
+      <c r="E7" s="14" t="s">
+        <v>12</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>8</v>
+      <c r="F7" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>13</v>
+      <c r="G7" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -1540,23 +1579,23 @@
     </row>
     <row r="8" spans="1:25" ht="169.50" customHeight="1">
       <c r="A8" s="7"/>
-      <c r="B8" s="10" t="n">
-        <v>45240</v>
+      <c r="B8" s="40" t="s">
+        <v>18</v>
       </c>
-      <c r="C8" s="11" t="n">
-        <v>0.691666666666666607</v>
+      <c r="C8" s="10" t="n">
+        <v>0.691666666666666519</v>
       </c>
-      <c r="D8" s="11" t="n">
+      <c r="D8" s="10" t="n">
         <v>0.708333333333333393</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>14</v>
+      <c r="F8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -1579,23 +1618,23 @@
     </row>
     <row r="9" spans="1:25" ht="123.75" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="14" t="n">
-        <v>45243</v>
+      <c r="B9" s="41" t="s">
+        <v>20</v>
       </c>
-      <c r="C9" s="15" t="n">
+      <c r="C9" s="13" t="n">
         <v>0.690972222222222232</v>
       </c>
-      <c r="D9" s="15" t="n">
+      <c r="D9" s="13" t="n">
         <v>0.708333333333333393</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>15</v>
+      <c r="E9" s="14" t="s">
+        <v>21</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>8</v>
+      <c r="F9" s="14" t="s">
+        <v>9</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>16</v>
+      <c r="G9" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1618,23 +1657,23 @@
     </row>
     <row r="10" spans="1:25" ht="115.50" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="44" t="n">
-        <v>45244</v>
+      <c r="B10" s="40" t="s">
+        <v>23</v>
       </c>
-      <c r="C10" s="11" t="n">
+      <c r="C10" s="10" t="n">
         <v>0.690972222222222232</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="D10" s="10" t="n">
         <v>0.743055555555555536</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>17</v>
+      <c r="F10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -1657,23 +1696,23 @@
     </row>
     <row r="11" spans="1:25" ht="148.50" customHeight="1">
       <c r="A11" s="7"/>
-      <c r="B11" s="45" t="n">
-        <v>45246</v>
+      <c r="B11" s="42" t="s">
+        <v>25</v>
       </c>
-      <c r="C11" s="20" t="n">
-        <v>0.416666666666666696</v>
+      <c r="C11" s="16" t="n">
+        <v>0.416666666666666607</v>
       </c>
-      <c r="D11" s="20" t="n">
+      <c r="D11" s="16" t="n">
         <v>0.430555555555555536</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>18</v>
+      <c r="F11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -1696,12 +1735,22 @@
     </row>
     <row r="12" spans="1:25" ht="108" customHeight="1">
       <c r="A12" s="7"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="38" t="n">
+        <v>45247</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0.416666666666666607</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>0.429166666666666607</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="12"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1723,12 +1772,24 @@
     </row>
     <row r="13" spans="1:25" ht="108.75" customHeight="1">
       <c r="A13" s="7"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
+      <c r="B13" s="39" t="n">
+        <v>45250</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>0.8125</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -1750,12 +1811,24 @@
     </row>
     <row r="14" spans="1:25" ht="114" customHeight="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>0.409722222222222321</v>
+      </c>
+      <c r="D14" s="10" t="n">
+        <v>0.430555555555555536</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -1777,12 +1850,24 @@
     </row>
     <row r="15" spans="1:25" ht="163.50" customHeight="1">
       <c r="A15" s="7"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="17"/>
+      <c r="B15" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="13" t="n">
+        <v>0.416666666666666607</v>
+      </c>
+      <c r="D15" s="13" t="n">
+        <v>0.430555555555555536</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -1804,12 +1889,24 @@
     </row>
     <row r="16" spans="1:25" ht="82.50" customHeight="1">
       <c r="A16" s="7"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="B16" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>0.416666666666666696</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>0.430555555555555536</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1831,12 +1928,12 @@
     </row>
     <row r="17" spans="1:25" ht="158.25" customHeight="1">
       <c r="A17" s="7"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="28"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="22"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -1858,12 +1955,12 @@
     </row>
     <row r="18" spans="1:25" ht="142.50" customHeight="1">
       <c r="A18" s="7"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="25"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -1885,12 +1982,12 @@
     </row>
     <row r="19" spans="1:25" ht="152.25" customHeight="1">
       <c r="A19" s="7"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="28"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1912,12 +2009,12 @@
     </row>
     <row r="20" spans="1:25" ht="135.75" customHeight="1">
       <c r="A20" s="7"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="25"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1939,12 +2036,12 @@
     </row>
     <row r="21" spans="1:25" ht="133.50" customHeight="1">
       <c r="A21" s="7"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="28"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1966,12 +2063,12 @@
     </row>
     <row r="22" spans="1:25" ht="122.25" customHeight="1">
       <c r="A22" s="7"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="25"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -1993,12 +2090,12 @@
     </row>
     <row r="23" spans="1:25" ht="114.75" customHeight="1">
       <c r="A23" s="7"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="28"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="22"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -2020,14 +2117,14 @@
     </row>
     <row r="24" spans="1:25" ht="96" customHeight="1">
       <c r="A24" s="7"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="34"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
@@ -2047,12 +2144,12 @@
     </row>
     <row r="25" spans="1:25" ht="108" customHeight="1">
       <c r="A25" s="7"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="28"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -2073,16 +2170,16 @@
       <c r="Y25" s="4"/>
     </row>
     <row r="26" spans="1:25" ht="72.75" customHeight="1">
-      <c r="A26" s="36"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
@@ -2100,16 +2197,16 @@
       <c r="Y26" s="4"/>
     </row>
     <row r="27" spans="1:25" ht="88.50" customHeight="1">
-      <c r="A27" s="36"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -2127,16 +2224,16 @@
       <c r="Y27" s="4"/>
     </row>
     <row r="28" spans="1:25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
@@ -2154,16 +2251,16 @@
       <c r="Y28" s="4"/>
     </row>
     <row r="29" spans="1:25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
@@ -2187,7 +2284,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
-      <c r="G30" s="40"/>
+      <c r="G30" s="34"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -2214,7 +2311,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
-      <c r="G31" s="40"/>
+      <c r="G31" s="34"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
@@ -2241,7 +2338,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="40"/>
+      <c r="G32" s="34"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
@@ -2268,7 +2365,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="40"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2295,7 +2392,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="40"/>
+      <c r="G34" s="34"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -2322,7 +2419,7 @@
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="40"/>
+      <c r="G35" s="34"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
@@ -2349,7 +2446,7 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
-      <c r="G36" s="40"/>
+      <c r="G36" s="34"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -2376,7 +2473,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
-      <c r="G37" s="40"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
@@ -2403,7 +2500,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="40"/>
+      <c r="G38" s="34"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -2430,7 +2527,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="40"/>
+      <c r="G39" s="34"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
@@ -2457,7 +2554,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
-      <c r="G40" s="40"/>
+      <c r="G40" s="34"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
@@ -2484,7 +2581,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="40"/>
+      <c r="G41" s="34"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
@@ -2511,7 +2608,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
-      <c r="G42" s="40"/>
+      <c r="G42" s="34"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -2538,7 +2635,7 @@
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="40"/>
+      <c r="G43" s="34"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
@@ -2565,7 +2662,7 @@
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
-      <c r="G44" s="40"/>
+      <c r="G44" s="34"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -2592,7 +2689,7 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
-      <c r="G45" s="40"/>
+      <c r="G45" s="34"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
@@ -2619,7 +2716,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
-      <c r="G46" s="40"/>
+      <c r="G46" s="34"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
@@ -2646,7 +2743,7 @@
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
-      <c r="G47" s="40"/>
+      <c r="G47" s="34"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="8"/>
@@ -28350,7 +28447,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1700239791" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1700834835" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -28359,17 +28456,17 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1700239791" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1700239791" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1700239791" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1700239791" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1700834835" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1700834835" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1700834835" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1700834835" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1700239791" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1700834835" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>